<commit_message>
added some graphs for the flow meter
</commit_message>
<xml_diff>
--- a/analysis/Flow Meter Calibration/BucketCalibrationValues.xlsx
+++ b/analysis/Flow Meter Calibration/BucketCalibrationValues.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jntil\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jntil\Documents\Git_Repos\liquid-engine-test-stand\analysis\Flow Meter Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C96AD79C-10AE-4098-8EDC-0F9F6481327D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3F2B17-17C4-440E-81E8-26291AB6DC97}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7425" xr2:uid="{84682937-0FE1-482E-9032-2C5AD32B1255}"/>
   </bookViews>
@@ -4151,16 +4151,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4189,16 +4189,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>428625</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4228,13 +4228,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>138112</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>442912</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4562,7 +4562,7 @@
   <dimension ref="B3:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4599,7 +4599,7 @@
         <v>0.5</v>
       </c>
       <c r="E6">
-        <f>B6/60</f>
+        <f t="shared" ref="E6:E16" si="0">B6/60</f>
         <v>2.8666666666666667E-2</v>
       </c>
     </row>
@@ -4614,7 +4614,7 @@
         <v>0.75</v>
       </c>
       <c r="E7">
-        <f>B7/60</f>
+        <f t="shared" si="0"/>
         <v>0.10400000000000001</v>
       </c>
     </row>
@@ -4629,7 +4629,7 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <f>B8/60</f>
+        <f t="shared" si="0"/>
         <v>0.13949999999999999</v>
       </c>
     </row>
@@ -4644,7 +4644,7 @@
         <v>1.25</v>
       </c>
       <c r="E9">
-        <f>B9/60</f>
+        <f t="shared" si="0"/>
         <v>0.18433333333333335</v>
       </c>
     </row>
@@ -4659,7 +4659,7 @@
         <v>1.5</v>
       </c>
       <c r="E10">
-        <f>B10/60</f>
+        <f t="shared" si="0"/>
         <v>0.2135</v>
       </c>
     </row>
@@ -4674,7 +4674,7 @@
         <v>1.75</v>
       </c>
       <c r="E11">
-        <f>B11/60</f>
+        <f t="shared" si="0"/>
         <v>0.24333333333333332</v>
       </c>
     </row>
@@ -4689,7 +4689,7 @@
         <v>2</v>
       </c>
       <c r="E12">
-        <f>B12/60</f>
+        <f t="shared" si="0"/>
         <v>0.28950000000000004</v>
       </c>
     </row>
@@ -4704,7 +4704,7 @@
         <v>2.25</v>
       </c>
       <c r="E13">
-        <f>B13/60</f>
+        <f t="shared" si="0"/>
         <v>0.31850000000000001</v>
       </c>
     </row>
@@ -4719,7 +4719,7 @@
         <v>2.5</v>
       </c>
       <c r="E14">
-        <f>B14/60</f>
+        <f t="shared" si="0"/>
         <v>0.36849999999999999</v>
       </c>
     </row>
@@ -4734,7 +4734,7 @@
         <v>2.75</v>
       </c>
       <c r="E15">
-        <f>B15/60</f>
+        <f t="shared" si="0"/>
         <v>0.41750000000000004</v>
       </c>
     </row>
@@ -4749,7 +4749,7 @@
         <v>3</v>
       </c>
       <c r="E16">
-        <f>B16/60</f>
+        <f t="shared" si="0"/>
         <v>0.46300000000000002</v>
       </c>
     </row>
@@ -4774,7 +4774,7 @@
         <v>0.75</v>
       </c>
       <c r="E21">
-        <f>B21/60</f>
+        <f t="shared" ref="E21:E30" si="1">B21/60</f>
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
@@ -4789,7 +4789,7 @@
         <v>1</v>
       </c>
       <c r="E22">
-        <f>B22/60</f>
+        <f t="shared" si="1"/>
         <v>0.13466666666666666</v>
       </c>
     </row>
@@ -4804,7 +4804,7 @@
         <v>1.25</v>
       </c>
       <c r="E23">
-        <f>B23/60</f>
+        <f t="shared" si="1"/>
         <v>0.16316666666666665</v>
       </c>
     </row>
@@ -4819,7 +4819,7 @@
         <v>1.5</v>
       </c>
       <c r="E24">
-        <f>B24/60</f>
+        <f t="shared" si="1"/>
         <v>0.18716666666666668</v>
       </c>
     </row>
@@ -4834,7 +4834,7 @@
         <v>1.75</v>
       </c>
       <c r="E25">
-        <f>B25/60</f>
+        <f t="shared" si="1"/>
         <v>0.22533333333333333</v>
       </c>
     </row>
@@ -4849,7 +4849,7 @@
         <v>2</v>
       </c>
       <c r="E26">
-        <f>B26/60</f>
+        <f t="shared" si="1"/>
         <v>0.25933333333333336</v>
       </c>
     </row>
@@ -4864,7 +4864,7 @@
         <v>2.25</v>
       </c>
       <c r="E27">
-        <f>B27/60</f>
+        <f t="shared" si="1"/>
         <v>0.29666666666666669</v>
       </c>
     </row>
@@ -4879,7 +4879,7 @@
         <v>2.5</v>
       </c>
       <c r="E28">
-        <f>B28/60</f>
+        <f t="shared" si="1"/>
         <v>0.33100000000000002</v>
       </c>
     </row>
@@ -4894,7 +4894,7 @@
         <v>2.75</v>
       </c>
       <c r="E29">
-        <f>B29/60</f>
+        <f t="shared" si="1"/>
         <v>0.3731666666666667</v>
       </c>
     </row>
@@ -4909,7 +4909,7 @@
         <v>3</v>
       </c>
       <c r="E30">
-        <f>B30/60</f>
+        <f t="shared" si="1"/>
         <v>0.41366666666666668</v>
       </c>
     </row>
@@ -4937,7 +4937,7 @@
         <v>0.75</v>
       </c>
       <c r="E34">
-        <f>B34/60</f>
+        <f t="shared" ref="E34:E44" si="2">B34/60</f>
         <v>2.5166666666666667E-2</v>
       </c>
     </row>
@@ -4952,7 +4952,7 @@
         <v>1</v>
       </c>
       <c r="E35">
-        <f>B35/60</f>
+        <f t="shared" si="2"/>
         <v>6.0666666666666667E-2</v>
       </c>
     </row>
@@ -4967,7 +4967,7 @@
         <v>1.25</v>
       </c>
       <c r="E36">
-        <f>B36/60</f>
+        <f t="shared" si="2"/>
         <v>9.4E-2</v>
       </c>
     </row>
@@ -4982,7 +4982,7 @@
         <v>1.5</v>
       </c>
       <c r="E37">
-        <f>B37/60</f>
+        <f t="shared" si="2"/>
         <v>0.12383333333333332</v>
       </c>
     </row>
@@ -4997,7 +4997,7 @@
         <v>1.75</v>
       </c>
       <c r="E38">
-        <f>B38/60</f>
+        <f t="shared" si="2"/>
         <v>0.15683333333333332</v>
       </c>
     </row>
@@ -5012,7 +5012,7 @@
         <v>2</v>
       </c>
       <c r="E39">
-        <f>B39/60</f>
+        <f t="shared" si="2"/>
         <v>0.18099999999999999</v>
       </c>
     </row>
@@ -5027,7 +5027,7 @@
         <v>2.25</v>
       </c>
       <c r="E40">
-        <f>B40/60</f>
+        <f t="shared" si="2"/>
         <v>0.20516666666666666</v>
       </c>
     </row>
@@ -5042,7 +5042,7 @@
         <v>2.5</v>
       </c>
       <c r="E41">
-        <f>B41/60</f>
+        <f t="shared" si="2"/>
         <v>0.23866666666666667</v>
       </c>
     </row>
@@ -5057,7 +5057,7 @@
         <v>2.75</v>
       </c>
       <c r="E42">
-        <f>B42/60</f>
+        <f t="shared" si="2"/>
         <v>0.26766666666666666</v>
       </c>
     </row>
@@ -5072,7 +5072,7 @@
         <v>3</v>
       </c>
       <c r="E43">
-        <f>B43/60</f>
+        <f t="shared" si="2"/>
         <v>0.30050000000000004</v>
       </c>
     </row>
@@ -5087,7 +5087,7 @@
         <v>3.25</v>
       </c>
       <c r="E44">
-        <f>B44/60</f>
+        <f t="shared" si="2"/>
         <v>0.33200000000000002</v>
       </c>
     </row>
@@ -5126,7 +5126,7 @@
         <v>0.75</v>
       </c>
       <c r="E49">
-        <f>B49/60</f>
+        <f t="shared" ref="E49:E59" si="3">B49/60</f>
         <v>2.5333333333333333E-2</v>
       </c>
     </row>
@@ -5141,7 +5141,7 @@
         <v>1</v>
       </c>
       <c r="E50">
-        <f>B50/60</f>
+        <f t="shared" si="3"/>
         <v>5.2166666666666667E-2</v>
       </c>
     </row>
@@ -5156,7 +5156,7 @@
         <v>1.25</v>
       </c>
       <c r="E51">
-        <f>B51/60</f>
+        <f t="shared" si="3"/>
         <v>0.10966666666666666</v>
       </c>
     </row>
@@ -5171,7 +5171,7 @@
         <v>1.5</v>
       </c>
       <c r="E52">
-        <f>B52/60</f>
+        <f t="shared" si="3"/>
         <v>0.14533333333333334</v>
       </c>
     </row>
@@ -5186,7 +5186,7 @@
         <v>1.75</v>
       </c>
       <c r="E53">
-        <f>B53/60</f>
+        <f t="shared" si="3"/>
         <v>0.18016666666666667</v>
       </c>
     </row>
@@ -5201,7 +5201,7 @@
         <v>2</v>
       </c>
       <c r="E54">
-        <f>B54/60</f>
+        <f t="shared" si="3"/>
         <v>0.20366666666666669</v>
       </c>
     </row>
@@ -5216,7 +5216,7 @@
         <v>2.25</v>
       </c>
       <c r="E55">
-        <f>B55/60</f>
+        <f t="shared" si="3"/>
         <v>0.23966666666666667</v>
       </c>
     </row>
@@ -5231,7 +5231,7 @@
         <v>2.5</v>
       </c>
       <c r="E56">
-        <f>B56/60</f>
+        <f t="shared" si="3"/>
         <v>0.26816666666666666</v>
       </c>
     </row>
@@ -5246,7 +5246,7 @@
         <v>2.75</v>
       </c>
       <c r="E57">
-        <f>B57/60</f>
+        <f t="shared" si="3"/>
         <v>0.30416666666666664</v>
       </c>
     </row>
@@ -5261,7 +5261,7 @@
         <v>3</v>
       </c>
       <c r="E58">
-        <f>B58/60</f>
+        <f t="shared" si="3"/>
         <v>0.35216666666666663</v>
       </c>
     </row>
@@ -5276,7 +5276,7 @@
         <v>3.25</v>
       </c>
       <c r="E59">
-        <f>B59/60</f>
+        <f t="shared" si="3"/>
         <v>0.39433333333333331</v>
       </c>
     </row>

</xml_diff>